<commit_message>
Added Lao support and fixed a few errors
</commit_message>
<xml_diff>
--- a/Frontend/Localized Strings-WsClient.xlsx
+++ b/Frontend/Localized Strings-WsClient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/256c97ba8ed48425/Documents/Projects/PBX/WebSocketExample/Frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{E56E5DB7-DCE6-4147-AE74-1FCC07CA3D14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{481BDC06-BB12-4F06-9A42-E94F3F6842AC}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{E56E5DB7-DCE6-4147-AE74-1FCC07CA3D14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B4EFF110-36F0-42EF-89A9-F8F43BE78B39}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ABC2DD07-3A85-4A65-872C-28279EB9CF19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABC2DD07-3A85-4A65-872C-28279EB9CF19}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="5" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="en-UK" sheetId="8" r:id="rId4"/>
     <sheet name="de-DE" sheetId="4" r:id="rId5"/>
     <sheet name="es" sheetId="9" r:id="rId6"/>
-    <sheet name="Cultures" sheetId="10" r:id="rId7"/>
+    <sheet name="lo" sheetId="11" r:id="rId7"/>
+    <sheet name="Cultures" sheetId="10" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5216" uniqueCount="2217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5227" uniqueCount="2222">
   <si>
     <t>Name</t>
   </si>
@@ -6716,6 +6717,21 @@
   </si>
   <si>
     <t>Chinese (Traditional) Legacy</t>
+  </si>
+  <si>
+    <t>ເຊື່ອມຕໍ່ແລ້ວ</t>
+  </si>
+  <si>
+    <t>ບໍ່ເຊື່ອມຕໍ່</t>
+  </si>
+  <si>
+    <t>ເກີດຄວາມຜິດພາດໃນການເຊື່ອມຕໍ່ກັບເຊີບເວີ</t>
+  </si>
+  <si>
+    <t>ໄດ້ຮັບ</t>
+  </si>
+  <si>
+    <t>ລັດ Websocket</t>
   </si>
 </sst>
 </file>
@@ -6814,6 +6830,7 @@
       <sheetName val="en-UK"/>
       <sheetName val="de-DE"/>
       <sheetName val="es"/>
+      <sheetName val="lo"/>
       <sheetName val="Cultures"/>
     </sheetNames>
     <sheetDataSet>
@@ -6832,6 +6849,9 @@
           <cell r="D1" t="str">
             <v>es</v>
           </cell>
+          <cell r="E1" t="str">
+            <v>lo</v>
+          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
@@ -6839,6 +6859,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7244,13 +7265,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9597F68-F138-45BD-8CE4-EEEA05FC7803}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7258,9 +7279,10 @@
     <col min="1" max="2" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7273,8 +7295,11 @@
       <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7287,8 +7312,11 @@
       <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -7301,8 +7329,11 @@
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -7315,8 +7346,11 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -7329,8 +7363,11 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -7342,6 +7379,9 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2221</v>
       </c>
     </row>
   </sheetData>
@@ -9446,6 +9486,529 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41A51CA-307B-4BC1-9E78-75B615715701}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="str" cm="1">
+        <f t="array" aca="1" ref="B1" ca="1">RIGHT(CELL("filename",A1),LEN(CELL("filename",A1))-FIND("]",CELL("filename",A1)))</f>
+        <v>lo</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6">
+        <f ca="1">MATCH(B1,[1]Translations!A1:O1,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>IF(Default!A2="","",Default!A2)</f>
+        <v>Connected</v>
+      </c>
+      <c r="B4" t="str">
+        <f ca="1">IF(A4="","",VLOOKUP(Default!B2,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v>ເຊື່ອມຕໍ່ແລ້ວ</v>
+      </c>
+      <c r="C4" t="str">
+        <f>IF(Default!C2="","",Default!C2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>IF(Default!A3="","",Default!A3)</f>
+        <v>NotConnected</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">IF(A5="","",VLOOKUP(Default!B3,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v>ບໍ່ເຊື່ອມຕໍ່</v>
+      </c>
+      <c r="C5" t="str">
+        <f>IF(Default!C3="","",Default!C3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>IF(Default!A4="","",Default!A4)</f>
+        <v>ConnectionErrorMessage</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1">IF(A6="","",VLOOKUP(Default!B4,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v>ເກີດຄວາມຜິດພາດໃນການເຊື່ອມຕໍ່ກັບເຊີບເວີ</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(Default!C4="","",Default!C4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>IF(Default!A5="","",Default!A5)</f>
+        <v>Received</v>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1">IF(A7="","",VLOOKUP(Default!B5,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v>ໄດ້ຮັບ</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(Default!C5="","",Default!C5)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>IF(Default!A6="","",Default!A6)</f>
+        <v>WebsocketState</v>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">IF(A8="","",VLOOKUP(Default!B6,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v>ລັດ Websocket</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IF(Default!C6="","",Default!C6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>IF(Default!A7="","",Default!A7)</f>
+        <v/>
+      </c>
+      <c r="B9" t="str">
+        <f>IF(A9="","",VLOOKUP(Default!B7,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <f>IF(Default!C7="","",Default!C7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>IF(Default!A8="","",Default!A8)</f>
+        <v/>
+      </c>
+      <c r="B10" t="str">
+        <f>IF(A10="","",VLOOKUP(Default!B8,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <f>IF(Default!C8="","",Default!C8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>IF(Default!A9="","",Default!A9)</f>
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <f>IF(A11="","",VLOOKUP(Default!B9,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <f>IF(Default!C9="","",Default!C9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>IF(Default!A10="","",Default!A10)</f>
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <f>IF(A12="","",VLOOKUP(Default!B10,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <f>IF(Default!C10="","",Default!C10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>IF(Default!A11="","",Default!A11)</f>
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <f>IF(A13="","",VLOOKUP(Default!B11,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <f>IF(Default!C11="","",Default!C11)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>IF(Default!A12="","",Default!A12)</f>
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <f>IF(A14="","",VLOOKUP(Default!B12,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <f>IF(Default!C12="","",Default!C12)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>IF(Default!A13="","",Default!A13)</f>
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(A15="","",VLOOKUP(Default!B13,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <f>IF(Default!C13="","",Default!C13)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>IF(Default!A14="","",Default!A14)</f>
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <f>IF(A16="","",VLOOKUP(Default!B14,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <f>IF(Default!C14="","",Default!C14)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>IF(Default!A15="","",Default!A15)</f>
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(A17="","",VLOOKUP(Default!B15,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <f>IF(Default!C15="","",Default!C15)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>IF(Default!A16="","",Default!A16)</f>
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <f>IF(A18="","",VLOOKUP(Default!B16,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <f>IF(Default!C16="","",Default!C16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>IF(Default!A17="","",Default!A17)</f>
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <f>IF(A19="","",VLOOKUP(Default!B17,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(Default!C17="","",Default!C17)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>IF(Default!A18="","",Default!A18)</f>
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <f>IF(A20="","",VLOOKUP(Default!B18,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <f>IF(Default!C18="","",Default!C18)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>IF(Default!A19="","",Default!A19)</f>
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <f>IF(A21="","",VLOOKUP(Default!B19,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <f>IF(Default!C19="","",Default!C19)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>IF(Default!A20="","",Default!A20)</f>
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <f>IF(A22="","",VLOOKUP(Default!B20,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(Default!C20="","",Default!C20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>IF(Default!A21="","",Default!A21)</f>
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(A23="","",VLOOKUP(Default!B21,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <f>IF(Default!C21="","",Default!C21)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>IF(Default!A22="","",Default!A22)</f>
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <f>IF(A24="","",VLOOKUP(Default!B22,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <f>IF(Default!C22="","",Default!C22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>IF(Default!A23="","",Default!A23)</f>
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <f>IF(A25="","",VLOOKUP(Default!B23,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C25" t="str">
+        <f>IF(Default!C23="","",Default!C23)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>IF(Default!A24="","",Default!A24)</f>
+        <v/>
+      </c>
+      <c r="B26" t="str">
+        <f>IF(A26="","",VLOOKUP(Default!B24,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C26" t="str">
+        <f>IF(Default!C24="","",Default!C24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>IF(Default!A25="","",Default!A25)</f>
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <f>IF(A27="","",VLOOKUP(Default!B25,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C27" t="str">
+        <f>IF(Default!C25="","",Default!C25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>IF(Default!A26="","",Default!A26)</f>
+        <v/>
+      </c>
+      <c r="B28" t="str">
+        <f>IF(A28="","",VLOOKUP(Default!B26,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C28" t="str">
+        <f>IF(Default!C26="","",Default!C26)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>IF(Default!A27="","",Default!A27)</f>
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <f>IF(A29="","",VLOOKUP(Default!B27,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C29" t="str">
+        <f>IF(Default!C27="","",Default!C27)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>IF(Default!A28="","",Default!A28)</f>
+        <v/>
+      </c>
+      <c r="B30" t="str">
+        <f>IF(A30="","",VLOOKUP(Default!B28,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C30" t="str">
+        <f>IF(Default!C28="","",Default!C28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>IF(Default!A29="","",Default!A29)</f>
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <f>IF(A31="","",VLOOKUP(Default!B29,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C31" t="str">
+        <f>IF(Default!C29="","",Default!C29)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>IF(Default!A30="","",Default!A30)</f>
+        <v/>
+      </c>
+      <c r="B32" t="str">
+        <f>IF(A32="","",VLOOKUP(Default!B30,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C32" t="str">
+        <f>IF(Default!C30="","",Default!C30)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>IF(Default!A31="","",Default!A31)</f>
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <f>IF(A33="","",VLOOKUP(Default!B31,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C33" t="str">
+        <f>IF(Default!C31="","",Default!C31)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>IF(Default!A32="","",Default!A32)</f>
+        <v/>
+      </c>
+      <c r="B34" t="str">
+        <f>IF(A34="","",VLOOKUP(Default!B32,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C34" t="str">
+        <f>IF(Default!C32="","",Default!C32)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>IF(Default!A33="","",Default!A33)</f>
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <f>IF(A35="","",VLOOKUP(Default!B33,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C35" t="str">
+        <f>IF(Default!C33="","",Default!C33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>IF(Default!A34="","",Default!A34)</f>
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <f>IF(A36="","",VLOOKUP(Default!B34,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C36" t="str">
+        <f>IF(Default!C34="","",Default!C34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>IF(Default!A35="","",Default!A35)</f>
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <f>IF(A37="","",VLOOKUP(Default!B35,Translations!$A$2:$F$100,$B$2,FALSE))</f>
+        <v/>
+      </c>
+      <c r="C37" t="str">
+        <f>IF(Default!C35="","",Default!C35)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95C58A5-CBB9-4945-B9B7-C5178E5DE09A}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F860"/>

</xml_diff>

<commit_message>
Fixed issue if the server terminated the connection. Updated Documentation
</commit_message>
<xml_diff>
--- a/Frontend/Localized Strings-WsClient.xlsx
+++ b/Frontend/Localized Strings-WsClient.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/256c97ba8ed48425/Documents/Projects/PBX/WebSocketExample/Frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{E56E5DB7-DCE6-4147-AE74-1FCC07CA3D14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B4EFF110-36F0-42EF-89A9-F8F43BE78B39}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{E56E5DB7-DCE6-4147-AE74-1FCC07CA3D14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C295299D-37BA-418A-819D-07BFA802F8D9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{ABC2DD07-3A85-4A65-872C-28279EB9CF19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABC2DD07-3A85-4A65-872C-28279EB9CF19}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="5" r:id="rId1"/>
@@ -7165,7 +7165,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9489,7 +9489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41A51CA-307B-4BC1-9E78-75B615715701}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>